<commit_message>
Removed dec_id for --TEST
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_VS.xlsx
+++ b/curation/draft/collection/collection_specialization_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A934A41-FEEA-E841-BFC2-17FDEF4AA82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74BCBEC-101C-EE4E-8A0E-0C5763531388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="349">
   <si>
     <t>package_date</t>
   </si>
@@ -1065,9 +1065,6 @@
   </si>
   <si>
     <t>C25208</t>
-  </si>
-  <si>
-    <t>C67153</t>
   </si>
   <si>
     <t>2-2</t>
@@ -1503,10 +1500,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="Y5" sqref="Y5"/>
+      <selection pane="bottomLeft" activeCell="M129" sqref="M129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1575,7 +1572,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>10</v>
@@ -1614,10 +1611,10 @@
         <v>21</v>
       </c>
       <c r="X1" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>348</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>22</v>
@@ -1886,7 +1883,7 @@
         <v>37</v>
       </c>
       <c r="Y5" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AC5"/>
       <c r="AG5" t="s">
@@ -2516,9 +2513,6 @@
       <c r="N15" t="s">
         <v>326</v>
       </c>
-      <c r="O15" t="s">
-        <v>343</v>
-      </c>
       <c r="Q15" t="s">
         <v>327</v>
       </c>
@@ -2898,9 +2892,6 @@
       <c r="N21" t="s">
         <v>326</v>
       </c>
-      <c r="O21" t="s">
-        <v>343</v>
-      </c>
       <c r="Q21" t="s">
         <v>327</v>
       </c>
@@ -3555,9 +3546,6 @@
       <c r="N31" t="s">
         <v>326</v>
       </c>
-      <c r="O31" t="s">
-        <v>343</v>
-      </c>
       <c r="Q31" t="s">
         <v>327</v>
       </c>
@@ -4423,9 +4411,6 @@
       <c r="N44" t="s">
         <v>326</v>
       </c>
-      <c r="O44" t="s">
-        <v>343</v>
-      </c>
       <c r="Q44" t="s">
         <v>327</v>
       </c>
@@ -5291,9 +5276,6 @@
       <c r="N57" t="s">
         <v>326</v>
       </c>
-      <c r="O57" t="s">
-        <v>343</v>
-      </c>
       <c r="Q57" t="s">
         <v>327</v>
       </c>
@@ -5946,9 +5928,6 @@
       <c r="N67" t="s">
         <v>326</v>
       </c>
-      <c r="O67" t="s">
-        <v>343</v>
-      </c>
       <c r="Q67" t="s">
         <v>327</v>
       </c>
@@ -6275,7 +6254,7 @@
         <v>64</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="R72">
         <v>3</v>
@@ -6792,9 +6771,6 @@
       <c r="N80" t="s">
         <v>326</v>
       </c>
-      <c r="O80" t="s">
-        <v>343</v>
-      </c>
       <c r="Q80" t="s">
         <v>327</v>
       </c>
@@ -7310,9 +7286,6 @@
       <c r="N88" t="s">
         <v>326</v>
       </c>
-      <c r="O88" t="s">
-        <v>343</v>
-      </c>
       <c r="Q88" t="s">
         <v>327</v>
       </c>
@@ -7826,9 +7799,6 @@
       <c r="N96" t="s">
         <v>326</v>
       </c>
-      <c r="O96" t="s">
-        <v>343</v>
-      </c>
       <c r="Q96" t="s">
         <v>327</v>
       </c>
@@ -8206,9 +8176,6 @@
       <c r="N102" t="s">
         <v>326</v>
       </c>
-      <c r="O102" t="s">
-        <v>343</v>
-      </c>
       <c r="Q102" t="s">
         <v>327</v>
       </c>
@@ -8583,7 +8550,7 @@
         <v>239</v>
       </c>
       <c r="E108" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G108" t="s">
         <v>33</v>
@@ -8657,9 +8624,6 @@
       </c>
       <c r="N109" t="s">
         <v>326</v>
-      </c>
-      <c r="O109" t="s">
-        <v>343</v>
       </c>
       <c r="Q109" t="s">
         <v>327</v>

</xml_diff>

<commit_message>
updates related to collection
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_VS.xlsx
+++ b/curation/draft/collection/collection_specialization_VS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74BCBEC-101C-EE4E-8A0E-0C5763531388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F275732F-3C72-4623-AB1A-A2E2EE77620F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_VS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="349">
   <si>
     <t>package_date</t>
   </si>
@@ -1501,46 +1501,46 @@
   <dimension ref="A1:AJ113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="M129" sqref="M129"/>
+      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" customWidth="1"/>
-    <col min="8" max="8" width="27.6640625" customWidth="1"/>
-    <col min="9" max="9" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
     <col min="10" max="11" width="19" customWidth="1"/>
     <col min="12" max="12" width="48" customWidth="1"/>
-    <col min="13" max="13" width="22.1640625" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" customWidth="1"/>
     <col min="15" max="15" width="16" customWidth="1"/>
     <col min="16" max="16" width="37" style="1" customWidth="1"/>
     <col min="17" max="17" width="37" customWidth="1"/>
     <col min="18" max="18" width="22" customWidth="1"/>
-    <col min="19" max="19" width="26.33203125" customWidth="1"/>
-    <col min="20" max="20" width="18.1640625" customWidth="1"/>
-    <col min="21" max="21" width="11.33203125" customWidth="1"/>
-    <col min="22" max="22" width="14.83203125" customWidth="1"/>
-    <col min="23" max="24" width="16.83203125" customWidth="1"/>
+    <col min="19" max="19" width="26.28515625" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" customWidth="1"/>
+    <col min="23" max="24" width="16.85546875" customWidth="1"/>
     <col min="25" max="25" width="29" customWidth="1"/>
-    <col min="26" max="26" width="14.5" customWidth="1"/>
-    <col min="27" max="27" width="19.83203125" customWidth="1"/>
+    <col min="26" max="26" width="14.42578125" customWidth="1"/>
+    <col min="27" max="27" width="19.85546875" customWidth="1"/>
     <col min="28" max="29" width="37" style="1" customWidth="1"/>
-    <col min="30" max="30" width="22.1640625" customWidth="1"/>
+    <col min="30" max="30" width="22.140625" customWidth="1"/>
     <col min="31" max="31" width="30" customWidth="1"/>
-    <col min="32" max="32" width="16.6640625" customWidth="1"/>
-    <col min="33" max="33" width="34.5" customWidth="1"/>
-    <col min="34" max="34" width="63.5" customWidth="1"/>
-    <col min="35" max="35" width="27.6640625" customWidth="1"/>
-    <col min="36" max="36" width="22.33203125" customWidth="1"/>
+    <col min="32" max="32" width="16.7109375" customWidth="1"/>
+    <col min="33" max="33" width="34.42578125" customWidth="1"/>
+    <col min="34" max="34" width="63.42578125" customWidth="1"/>
+    <col min="35" max="35" width="27.7109375" customWidth="1"/>
+    <col min="36" max="36" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" t="s">
         <v>35</v>
@@ -1716,7 +1716,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>35</v>
@@ -1768,7 +1768,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>45</v>
@@ -1826,7 +1826,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>45</v>
@@ -1893,7 +1893,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>45</v>
@@ -1966,7 +1966,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>60</v>
@@ -2024,7 +2024,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>60</v>
@@ -2059,6 +2059,9 @@
       <c r="O8" t="s">
         <v>97</v>
       </c>
+      <c r="P8" s="1" t="s">
+        <v>250</v>
+      </c>
       <c r="R8">
         <v>2</v>
       </c>
@@ -2093,7 +2096,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>60</v>
@@ -2165,7 +2168,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>60</v>
@@ -2200,6 +2203,9 @@
       <c r="O10" t="s">
         <v>50</v>
       </c>
+      <c r="P10" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="R10">
         <v>4</v>
       </c>
@@ -2220,7 +2226,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>60</v>
@@ -2290,7 +2296,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>79</v>
@@ -2348,7 +2354,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>79</v>
@@ -2423,7 +2429,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
         <v>79</v>
@@ -2481,7 +2487,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>45</v>
@@ -2542,7 +2548,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>79</v>
@@ -2614,7 +2620,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>87</v>
@@ -2669,7 +2675,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>87</v>
@@ -2730,7 +2736,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
         <v>87</v>
@@ -2802,7 +2808,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" t="s">
         <v>87</v>
@@ -2860,7 +2866,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>87</v>
@@ -2921,7 +2927,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
         <v>87</v>
@@ -2982,7 +2988,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
         <v>87</v>
@@ -3054,7 +3060,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" t="s">
         <v>94</v>
@@ -3112,7 +3118,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" t="s">
         <v>94</v>
@@ -3184,7 +3190,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" t="s">
         <v>94</v>
@@ -3256,7 +3262,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
         <v>94</v>
@@ -3328,7 +3334,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" t="s">
         <v>94</v>
@@ -3386,7 +3392,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" t="s">
         <v>94</v>
@@ -3456,7 +3462,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" t="s">
         <v>94</v>
@@ -3514,7 +3520,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" t="s">
         <v>94</v>
@@ -3575,7 +3581,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" t="s">
         <v>94</v>
@@ -3647,7 +3653,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" t="s">
         <v>94</v>
@@ -3719,7 +3725,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" t="s">
         <v>94</v>
@@ -3791,7 +3797,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" t="s">
         <v>94</v>
@@ -3849,7 +3855,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" t="s">
         <v>94</v>
@@ -3919,7 +3925,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" t="s">
         <v>121</v>
@@ -3977,7 +3983,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" t="s">
         <v>121</v>
@@ -4047,7 +4053,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" t="s">
         <v>139</v>
@@ -4119,7 +4125,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" t="s">
         <v>121</v>
@@ -4191,7 +4197,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" t="s">
         <v>121</v>
@@ -4252,7 +4258,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" t="s">
         <v>121</v>
@@ -4321,7 +4327,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" t="s">
         <v>121</v>
@@ -4379,7 +4385,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" t="s">
         <v>121</v>
@@ -4440,7 +4446,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" t="s">
         <v>121</v>
@@ -4510,7 +4516,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="46" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" t="s">
         <v>121</v>
@@ -4582,7 +4588,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="47" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" t="s">
         <v>121</v>
@@ -4654,7 +4660,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" t="s">
         <v>121</v>
@@ -4712,7 +4718,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" t="s">
         <v>121</v>
@@ -4781,7 +4787,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" t="s">
         <v>139</v>
@@ -4839,7 +4845,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" t="s">
         <v>139</v>
@@ -4911,7 +4917,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="52" spans="1:34" ht="48" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:34" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" t="s">
         <v>139</v>
@@ -4983,7 +4989,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="53" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" t="s">
         <v>139</v>
@@ -5055,7 +5061,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" t="s">
         <v>139</v>
@@ -5116,7 +5122,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" t="s">
         <v>139</v>
@@ -5186,7 +5192,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="56" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" t="s">
         <v>158</v>
@@ -5244,7 +5250,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" t="s">
         <v>158</v>
@@ -5305,7 +5311,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="58" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" t="s">
         <v>139</v>
@@ -5377,7 +5383,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="59" spans="1:34" ht="48" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:34" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" t="s">
         <v>139</v>
@@ -5449,7 +5455,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="60" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:34" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" t="s">
         <v>139</v>
@@ -5521,7 +5527,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="61" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" t="s">
         <v>139</v>
@@ -5582,7 +5588,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" t="s">
         <v>139</v>
@@ -5652,7 +5658,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" t="s">
         <v>149</v>
@@ -5710,7 +5716,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" t="s">
         <v>149</v>
@@ -5768,7 +5774,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" t="s">
         <v>149</v>
@@ -5838,7 +5844,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="66" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" t="s">
         <v>149</v>
@@ -5896,7 +5902,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" t="s">
         <v>149</v>
@@ -5957,7 +5963,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="68" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" t="s">
         <v>149</v>
@@ -6018,7 +6024,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="69" spans="1:34" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:34" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" t="s">
         <v>149</v>
@@ -6088,7 +6094,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="70" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" t="s">
         <v>158</v>
@@ -6146,7 +6152,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:34" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" t="s">
         <v>158</v>
@@ -6218,7 +6224,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="72" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:34" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" t="s">
         <v>158</v>
@@ -6290,7 +6296,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" t="s">
         <v>158</v>
@@ -6348,7 +6354,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="74" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" t="s">
         <v>60</v>
@@ -6418,7 +6424,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" t="s">
         <v>165</v>
@@ -6476,7 +6482,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" t="s">
         <v>165</v>
@@ -6537,7 +6543,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="77" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" t="s">
         <v>165</v>
@@ -6609,7 +6615,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" t="s">
         <v>165</v>
@@ -6681,7 +6687,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" t="s">
         <v>165</v>
@@ -6739,7 +6745,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" t="s">
         <v>165</v>
@@ -6800,7 +6806,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="81" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" t="s">
         <v>165</v>
@@ -6861,7 +6867,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="82" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" t="s">
         <v>165</v>
@@ -6933,7 +6939,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="83" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" t="s">
         <v>165</v>
@@ -7005,7 +7011,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" t="s">
         <v>181</v>
@@ -7063,7 +7069,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" t="s">
         <v>181</v>
@@ -7124,7 +7130,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="86" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" t="s">
         <v>181</v>
@@ -7196,7 +7202,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="87" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" t="s">
         <v>181</v>
@@ -7254,7 +7260,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" t="s">
         <v>181</v>
@@ -7315,7 +7321,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="89" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" t="s">
         <v>181</v>
@@ -7376,7 +7382,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="90" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" t="s">
         <v>181</v>
@@ -7448,7 +7454,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" t="s">
         <v>190</v>
@@ -7506,7 +7512,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" t="s">
         <v>190</v>
@@ -7576,7 +7582,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="93" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" t="s">
         <v>190</v>
@@ -7637,7 +7643,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="94" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" t="s">
         <v>190</v>
@@ -7709,7 +7715,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="95" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" t="s">
         <v>190</v>
@@ -7767,7 +7773,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="96" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" t="s">
         <v>190</v>
@@ -7828,7 +7834,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" t="s">
         <v>190</v>
@@ -7898,7 +7904,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="98" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" t="s">
         <v>190</v>
@@ -7959,7 +7965,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="99" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" t="s">
         <v>190</v>
@@ -8031,7 +8037,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="100" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" t="s">
         <v>60</v>
@@ -8089,7 +8095,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" t="s">
         <v>60</v>
@@ -8144,7 +8150,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="102" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" t="s">
         <v>60</v>
@@ -8205,7 +8211,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="103" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" t="s">
         <v>60</v>
@@ -8277,7 +8283,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="104" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:34" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" t="s">
         <v>60</v>
@@ -8349,7 +8355,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="105" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" t="s">
         <v>60</v>
@@ -8410,7 +8416,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="106" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" t="s">
         <v>60</v>
@@ -8480,7 +8486,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="107" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" t="s">
         <v>158</v>
@@ -8538,7 +8544,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" t="s">
         <v>60</v>
@@ -8593,7 +8599,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="109" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" t="s">
         <v>158</v>
@@ -8654,7 +8660,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="110" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" t="s">
         <v>158</v>
@@ -8726,7 +8732,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="111" spans="1:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:34" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" t="s">
         <v>158</v>
@@ -8798,7 +8804,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="112" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" t="s">
         <v>158</v>
@@ -8859,7 +8865,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="113" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" t="s">
         <v>158</v>

</xml_diff>